<commit_message>
Prueba interfaz de Colaboradores
</commit_message>
<xml_diff>
--- a/test_colaboradores.xlsx
+++ b/test_colaboradores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cosas que no quiero ver en el escritorio\Eternal Damnation\TEC 2023\VERANO\Proyecto de Software\proyecto-gestor-turnos-semanal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE7F3BA-CDB6-4538-A81B-F399CC8A6020}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D7ADC-E8F2-4977-BD16-751F34C295C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -108,9 +108,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -395,105 +397,106 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>22562222</v>
       </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="D2" s="2">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="1">
         <v>22841756</v>
       </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
+      </c>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="1">
         <v>23695478</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
+      </c>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
+      <c r="G4" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Datos de colaboradores DB y correccion en controlador
</commit_message>
<xml_diff>
--- a/test_colaboradores.xlsx
+++ b/test_colaboradores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\cosas que no quiero ver en el escritorio\Eternal Damnation\TEC 2023\VERANO\Proyecto de Software\proyecto-gestor-turnos-semanal\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc89e812a8d50f8a/Escritorio/proyecto-gestor-turnos-semanal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC5D7ADC-E8F2-4977-BD16-751F34C295C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{BC5D7ADC-E8F2-4977-BD16-751F34C295C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F80466DC-A9D4-4ECE-8824-48971A039AAC}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31995" yWindow="900" windowWidth="14400" windowHeight="7275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -397,18 +397,18 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="9.140625" style="2"/>
+    <col min="4" max="7" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -431,7 +431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -442,7 +442,7 @@
         <v>22562222</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -454,7 +454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -465,19 +465,19 @@
         <v>22841756</v>
       </c>
       <c r="D3" s="2">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
       </c>
       <c r="F3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G3" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
@@ -488,13 +488,13 @@
         <v>23695478</v>
       </c>
       <c r="D4" s="2">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="E4" s="2">
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G4" s="2">
         <v>1</v>

</xml_diff>